<commit_message>
creation des pages admin pour populer les DB inventaire
</commit_message>
<xml_diff>
--- a/public/csv/inventory/test2.xlsx
+++ b/public/csv/inventory/test2.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="126">
   <si>
     <t>Localisation</t>
   </si>
@@ -57,9 +57,6 @@
   </si>
   <si>
     <t>PAQUET DE 3,06M2 - DIM 1288X198X7MM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">               </t>
   </si>
   <si>
     <t>M2</t>
@@ -788,11 +785,8 @@
       <c r="D2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -800,19 +794,16 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>17</v>
       </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
       <c r="G3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -820,19 +811,16 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
         <v>19</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>20</v>
       </c>
-      <c r="D4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -840,19 +828,16 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
         <v>22</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>23</v>
       </c>
-      <c r="D5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" t="s">
-        <v>14</v>
-      </c>
       <c r="G5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -860,19 +845,16 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
         <v>25</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>26</v>
       </c>
-      <c r="D6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" t="s">
-        <v>14</v>
-      </c>
       <c r="G6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -880,19 +862,16 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
         <v>28</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>29</v>
       </c>
-      <c r="D7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" t="s">
-        <v>14</v>
-      </c>
       <c r="G7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -900,19 +879,16 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
         <v>32</v>
       </c>
-      <c r="C8" t="s">
-        <v>33</v>
-      </c>
       <c r="D8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="G8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -920,19 +896,16 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" t="s">
         <v>34</v>
-      </c>
-      <c r="C9" t="s">
-        <v>35</v>
       </c>
       <c r="D9" t="s">
         <v>13</v>
       </c>
-      <c r="E9" t="s">
-        <v>14</v>
-      </c>
       <c r="G9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -940,19 +913,16 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" t="s">
         <v>36</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>37</v>
       </c>
-      <c r="D10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E10" t="s">
-        <v>14</v>
-      </c>
       <c r="G10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -960,19 +930,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" t="s">
         <v>39</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>40</v>
       </c>
-      <c r="D11" t="s">
-        <v>41</v>
-      </c>
-      <c r="E11" t="s">
-        <v>14</v>
-      </c>
       <c r="G11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -980,19 +947,16 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" t="s">
         <v>42</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>43</v>
       </c>
-      <c r="D12" t="s">
+      <c r="G12" t="s">
         <v>44</v>
-      </c>
-      <c r="E12" t="s">
-        <v>14</v>
-      </c>
-      <c r="G12" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -1000,19 +964,16 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" t="s">
         <v>46</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>47</v>
       </c>
-      <c r="D13" t="s">
-        <v>48</v>
-      </c>
-      <c r="E13" t="s">
-        <v>14</v>
-      </c>
       <c r="G13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -1020,19 +981,16 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" t="s">
         <v>49</v>
       </c>
-      <c r="C14" t="s">
-        <v>50</v>
-      </c>
       <c r="D14" t="s">
-        <v>30</v>
-      </c>
-      <c r="E14" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="G14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -1040,19 +998,16 @@
         <v>10</v>
       </c>
       <c r="B15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" t="s">
         <v>51</v>
       </c>
-      <c r="C15" t="s">
-        <v>52</v>
-      </c>
       <c r="D15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E15" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="G15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1060,19 +1015,16 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" t="s">
         <v>53</v>
       </c>
-      <c r="C16" t="s">
-        <v>54</v>
-      </c>
       <c r="D16" t="s">
-        <v>24</v>
-      </c>
-      <c r="E16" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="G16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1080,19 +1032,16 @@
         <v>10</v>
       </c>
       <c r="B17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" t="s">
         <v>55</v>
       </c>
-      <c r="C17" t="s">
-        <v>56</v>
-      </c>
       <c r="D17" t="s">
-        <v>30</v>
-      </c>
-      <c r="E17" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="G17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1100,19 +1049,16 @@
         <v>10</v>
       </c>
       <c r="B18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" t="s">
         <v>57</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>58</v>
       </c>
-      <c r="D18" t="s">
-        <v>59</v>
-      </c>
-      <c r="E18" t="s">
-        <v>14</v>
-      </c>
       <c r="G18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1120,19 +1066,16 @@
         <v>10</v>
       </c>
       <c r="B19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" t="s">
         <v>60</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>61</v>
       </c>
-      <c r="D19" t="s">
-        <v>62</v>
-      </c>
-      <c r="E19" t="s">
-        <v>14</v>
-      </c>
       <c r="G19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1143,16 +1086,13 @@
         <v>30313120</v>
       </c>
       <c r="C20" t="s">
+        <v>62</v>
+      </c>
+      <c r="D20" t="s">
         <v>63</v>
       </c>
-      <c r="D20" t="s">
+      <c r="G20" t="s">
         <v>64</v>
-      </c>
-      <c r="E20" t="s">
-        <v>14</v>
-      </c>
-      <c r="G20" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1160,19 +1100,16 @@
         <v>10</v>
       </c>
       <c r="B21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21" t="s">
         <v>66</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>67</v>
       </c>
-      <c r="D21" t="s">
-        <v>68</v>
-      </c>
-      <c r="E21" t="s">
-        <v>14</v>
-      </c>
       <c r="G21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1180,19 +1117,16 @@
         <v>10</v>
       </c>
       <c r="B22" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" t="s">
         <v>69</v>
-      </c>
-      <c r="C22" t="s">
-        <v>70</v>
       </c>
       <c r="D22" t="s">
         <v>13</v>
       </c>
-      <c r="E22" t="s">
-        <v>14</v>
-      </c>
       <c r="G22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1200,19 +1134,16 @@
         <v>10</v>
       </c>
       <c r="B23" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" t="s">
         <v>71</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>72</v>
       </c>
-      <c r="D23" t="s">
-        <v>73</v>
-      </c>
-      <c r="E23" t="s">
-        <v>14</v>
-      </c>
       <c r="G23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -1220,19 +1151,16 @@
         <v>10</v>
       </c>
       <c r="B24" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24" t="s">
         <v>74</v>
-      </c>
-      <c r="C24" t="s">
-        <v>75</v>
       </c>
       <c r="D24" t="s">
         <v>13</v>
       </c>
-      <c r="E24" t="s">
-        <v>14</v>
-      </c>
       <c r="G24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1240,19 +1168,16 @@
         <v>10</v>
       </c>
       <c r="B25" t="s">
+        <v>75</v>
+      </c>
+      <c r="C25" t="s">
         <v>76</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>77</v>
       </c>
-      <c r="D25" t="s">
-        <v>78</v>
-      </c>
-      <c r="E25" t="s">
-        <v>14</v>
-      </c>
       <c r="G25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -1260,19 +1185,16 @@
         <v>10</v>
       </c>
       <c r="B26" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26" t="s">
         <v>79</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>80</v>
       </c>
-      <c r="D26" t="s">
-        <v>81</v>
-      </c>
-      <c r="E26" t="s">
-        <v>14</v>
-      </c>
       <c r="G26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1280,19 +1202,16 @@
         <v>10</v>
       </c>
       <c r="B27" t="s">
+        <v>81</v>
+      </c>
+      <c r="C27" t="s">
         <v>82</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>83</v>
       </c>
-      <c r="D27" t="s">
-        <v>84</v>
-      </c>
-      <c r="E27" t="s">
-        <v>14</v>
-      </c>
       <c r="G27" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1300,19 +1219,16 @@
         <v>10</v>
       </c>
       <c r="B28" t="s">
+        <v>84</v>
+      </c>
+      <c r="C28" t="s">
         <v>85</v>
       </c>
-      <c r="C28" t="s">
-        <v>86</v>
-      </c>
       <c r="D28" t="s">
-        <v>21</v>
-      </c>
-      <c r="E28" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="G28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -1320,19 +1236,16 @@
         <v>10</v>
       </c>
       <c r="B29" t="s">
+        <v>86</v>
+      </c>
+      <c r="C29" t="s">
         <v>87</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>88</v>
       </c>
-      <c r="D29" t="s">
-        <v>89</v>
-      </c>
-      <c r="E29" t="s">
-        <v>14</v>
-      </c>
       <c r="G29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -1340,19 +1253,16 @@
         <v>10</v>
       </c>
       <c r="B30" t="s">
+        <v>89</v>
+      </c>
+      <c r="C30" t="s">
         <v>90</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>91</v>
       </c>
-      <c r="D30" t="s">
-        <v>92</v>
-      </c>
-      <c r="E30" t="s">
-        <v>14</v>
-      </c>
       <c r="G30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -1360,19 +1270,16 @@
         <v>10</v>
       </c>
       <c r="B31" t="s">
+        <v>92</v>
+      </c>
+      <c r="C31" t="s">
         <v>93</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>94</v>
       </c>
-      <c r="D31" t="s">
-        <v>95</v>
-      </c>
-      <c r="E31" t="s">
-        <v>14</v>
-      </c>
       <c r="G31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -1380,19 +1287,16 @@
         <v>10</v>
       </c>
       <c r="B32" t="s">
+        <v>95</v>
+      </c>
+      <c r="C32" t="s">
         <v>96</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>97</v>
       </c>
-      <c r="D32" t="s">
-        <v>98</v>
-      </c>
-      <c r="E32" t="s">
-        <v>14</v>
-      </c>
       <c r="G32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -1400,19 +1304,16 @@
         <v>10</v>
       </c>
       <c r="B33" t="s">
+        <v>98</v>
+      </c>
+      <c r="C33" t="s">
         <v>99</v>
       </c>
-      <c r="C33" t="s">
-        <v>100</v>
-      </c>
       <c r="D33" t="s">
-        <v>30</v>
-      </c>
-      <c r="E33" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="G33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -1420,19 +1321,16 @@
         <v>10</v>
       </c>
       <c r="B34" t="s">
+        <v>100</v>
+      </c>
+      <c r="C34" t="s">
         <v>101</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>102</v>
       </c>
-      <c r="D34" t="s">
-        <v>103</v>
-      </c>
-      <c r="E34" t="s">
-        <v>14</v>
-      </c>
       <c r="G34" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -1440,19 +1338,16 @@
         <v>10</v>
       </c>
       <c r="B35" t="s">
+        <v>103</v>
+      </c>
+      <c r="C35" t="s">
         <v>104</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>105</v>
       </c>
-      <c r="D35" t="s">
-        <v>106</v>
-      </c>
-      <c r="E35" t="s">
-        <v>14</v>
-      </c>
       <c r="G35" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -1460,19 +1355,16 @@
         <v>10</v>
       </c>
       <c r="B36" t="s">
+        <v>106</v>
+      </c>
+      <c r="C36" t="s">
         <v>107</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>108</v>
       </c>
-      <c r="D36" t="s">
-        <v>109</v>
-      </c>
-      <c r="E36" t="s">
-        <v>14</v>
-      </c>
       <c r="G36" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -1480,19 +1372,16 @@
         <v>10</v>
       </c>
       <c r="B37" t="s">
+        <v>109</v>
+      </c>
+      <c r="C37" t="s">
         <v>110</v>
       </c>
-      <c r="C37" t="s">
-        <v>111</v>
-      </c>
       <c r="D37" t="s">
-        <v>81</v>
-      </c>
-      <c r="E37" t="s">
-        <v>14</v>
+        <v>80</v>
       </c>
       <c r="G37" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -1500,19 +1389,16 @@
         <v>10</v>
       </c>
       <c r="B38" t="s">
+        <v>111</v>
+      </c>
+      <c r="C38" t="s">
         <v>112</v>
       </c>
-      <c r="C38" t="s">
-        <v>113</v>
-      </c>
       <c r="D38" t="s">
-        <v>30</v>
-      </c>
-      <c r="E38" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="G38" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -1520,19 +1406,16 @@
         <v>10</v>
       </c>
       <c r="B39" t="s">
+        <v>113</v>
+      </c>
+      <c r="C39" t="s">
         <v>114</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>115</v>
       </c>
-      <c r="D39" t="s">
-        <v>116</v>
-      </c>
-      <c r="E39" t="s">
-        <v>14</v>
-      </c>
       <c r="G39" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -1540,19 +1423,16 @@
         <v>10</v>
       </c>
       <c r="B40" t="s">
+        <v>116</v>
+      </c>
+      <c r="C40" t="s">
         <v>117</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>118</v>
       </c>
-      <c r="D40" t="s">
-        <v>119</v>
-      </c>
-      <c r="E40" t="s">
-        <v>14</v>
-      </c>
       <c r="G40" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -1560,19 +1440,16 @@
         <v>10</v>
       </c>
       <c r="B41" t="s">
+        <v>119</v>
+      </c>
+      <c r="C41" t="s">
         <v>120</v>
       </c>
-      <c r="C41" t="s">
-        <v>121</v>
-      </c>
       <c r="D41" t="s">
-        <v>48</v>
-      </c>
-      <c r="E41" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="G41" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -1580,19 +1457,16 @@
         <v>10</v>
       </c>
       <c r="B42" t="s">
+        <v>121</v>
+      </c>
+      <c r="C42" t="s">
         <v>122</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
         <v>123</v>
       </c>
-      <c r="D42" t="s">
-        <v>124</v>
-      </c>
-      <c r="E42" t="s">
-        <v>14</v>
-      </c>
       <c r="G42" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -1600,19 +1474,16 @@
         <v>10</v>
       </c>
       <c r="B43" t="s">
+        <v>124</v>
+      </c>
+      <c r="C43" t="s">
         <v>125</v>
       </c>
-      <c r="C43" t="s">
-        <v>126</v>
-      </c>
       <c r="D43" t="s">
-        <v>30</v>
-      </c>
-      <c r="E43" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="G43" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
gestion affichage article locations multiple | insert or update DB
</commit_message>
<xml_diff>
--- a/public/csv/inventory/test2.xlsx
+++ b/public/csv/inventory/test2.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="167">
   <si>
     <t>Localisation</t>
   </si>
@@ -47,7 +47,220 @@
     <t>Compt 2</t>
   </si>
   <si>
-    <t>A1 01</t>
+    <t>A1 01 A12 01</t>
+  </si>
+  <si>
+    <t>012655</t>
+  </si>
+  <si>
+    <t>BLOC PORTE ISOLANT CL B 67X56 93X204 GP</t>
+  </si>
+  <si>
+    <t>CHANT DROIT S3PT PERF+ AXE 50 JB FILME</t>
+  </si>
+  <si>
+    <t>UN</t>
+  </si>
+  <si>
+    <t>A1 01 A13 01</t>
+  </si>
+  <si>
+    <t>012656</t>
+  </si>
+  <si>
+    <t>BLOC PORTE ISOLANT CL B 67X56 93X204 DP</t>
+  </si>
+  <si>
+    <t>A1 01 B02 01</t>
+  </si>
+  <si>
+    <t>008229</t>
+  </si>
+  <si>
+    <t>SOUS COUCHE ISOLSOUND HD+ 2 MM 18 DB</t>
+  </si>
+  <si>
+    <t>ROULEAU DE 7,50M2REF3393 POLYANE INTEGRE</t>
+  </si>
+  <si>
+    <t>RL(X)</t>
+  </si>
+  <si>
+    <t>A1 01 B05 03</t>
+  </si>
+  <si>
+    <t>009247</t>
+  </si>
+  <si>
+    <t>MODULAR ONE CHENE PURE TEXTURE BOIS</t>
+  </si>
+  <si>
+    <t>PQT DE 2,493M2 DIM1285X194X8MM PARADOR</t>
+  </si>
+  <si>
+    <t>M2</t>
+  </si>
+  <si>
+    <t>A1 01 B06 01</t>
+  </si>
+  <si>
+    <t>006700</t>
+  </si>
+  <si>
+    <t>STRATIFIE BASIC 400V CHENE POLI TEXT M S</t>
+  </si>
+  <si>
+    <t>REF1426542 PAQUET DE 2,493M2 PARADOR</t>
+  </si>
+  <si>
+    <t>A1 01 B06 02</t>
+  </si>
+  <si>
+    <t>007356</t>
+  </si>
+  <si>
+    <t>STRATIFIE BASIC 400V CHENE HORIZON NATUR</t>
+  </si>
+  <si>
+    <t>REF1593797 PAQUET DE 2,493M2 PARADOR</t>
+  </si>
+  <si>
+    <t>A1 01 B07 01</t>
+  </si>
+  <si>
+    <t>012918</t>
+  </si>
+  <si>
+    <t>SOL STRATIFIE LD250 CHENE CAMPAGN 6843</t>
+  </si>
+  <si>
+    <t>PAQUET DE 1,70M2 - DIM 1287X220X10 MM</t>
+  </si>
+  <si>
+    <t>A1 01 B09 01</t>
+  </si>
+  <si>
+    <t>004864</t>
+  </si>
+  <si>
+    <t>PARQUET LOFT MOUNT CHENE APENNINES RU/CA</t>
+  </si>
+  <si>
+    <t>PAQUET DE 2,075M2 1820X190X14 HUILE GO4</t>
+  </si>
+  <si>
+    <t>A1 01 B10 01</t>
+  </si>
+  <si>
+    <t>006852</t>
+  </si>
+  <si>
+    <t>PARQUET LOFT PRO CHENE RU BROSSE VERNI</t>
+  </si>
+  <si>
+    <t>PQT DE 1,914M2 145X12X600-2200 G02 R+L</t>
+  </si>
+  <si>
+    <t>A1 01 B11 01</t>
+  </si>
+  <si>
+    <t>009248</t>
+  </si>
+  <si>
+    <t>PARQUET LOFT PRO CHENE ARZON RU/CA HUIL</t>
+  </si>
+  <si>
+    <t>180X12X1000-2000 PAQT 2,376M2 INCOLORE</t>
+  </si>
+  <si>
+    <t>A1 01 B12 01</t>
+  </si>
+  <si>
+    <t>012653</t>
+  </si>
+  <si>
+    <t>BLOC PORTE ISOLANT CL B 67X56 83X204 GP</t>
+  </si>
+  <si>
+    <t>A1 01 B13 01</t>
+  </si>
+  <si>
+    <t>012654</t>
+  </si>
+  <si>
+    <t>BLOC PORTE ISOLANT CL B 67X56 83X204 DP</t>
+  </si>
+  <si>
+    <t>A1 01 C02 02</t>
+  </si>
+  <si>
+    <t>BANDES PHALTEX 1200X48X10 MM</t>
+  </si>
+  <si>
+    <t>PAQUET DE 50 BANDES STEICO</t>
+  </si>
+  <si>
+    <t>PQT</t>
+  </si>
+  <si>
+    <t>A1 01 C05 01</t>
+  </si>
+  <si>
+    <t>020494</t>
+  </si>
+  <si>
+    <t>ESCALIER ESCAMOTABLE ECOWOOD40 120X60</t>
+  </si>
+  <si>
+    <t>HTMAX=2M84 TRAPPE 40 MM CAISSON U :</t>
+  </si>
+  <si>
+    <t>A1 01 C05 02</t>
+  </si>
+  <si>
+    <t>013741</t>
+  </si>
+  <si>
+    <t>ESCALIER ESCAMOTABLE ECOWOOD36 140X70</t>
+  </si>
+  <si>
+    <t>HTMAX=2M80 TRAPPE 36 MM CAISSON U :</t>
+  </si>
+  <si>
+    <t>A1 01 C06 01</t>
+  </si>
+  <si>
+    <t>006698</t>
+  </si>
+  <si>
+    <t>STRATIFIE BASIC 400V CHENE GRIS LUMIERE</t>
+  </si>
+  <si>
+    <t>REF1426530 PAQUET DE 2,493M2 PARADOR</t>
+  </si>
+  <si>
+    <t>A1 01 C06 02</t>
+  </si>
+  <si>
+    <t>010427</t>
+  </si>
+  <si>
+    <t>MODULAR ONE CHENE URBAN CHAULE GRIS</t>
+  </si>
+  <si>
+    <t>A1 01 C06 03</t>
+  </si>
+  <si>
+    <t>014537</t>
+  </si>
+  <si>
+    <t>VINYLE RD300S 7326 CHENE BH 228X1290X5,5</t>
+  </si>
+  <si>
+    <t>REF5941007326 PAQUET DE 2,06M2 MEISTER</t>
+  </si>
+  <si>
+    <t>A1 01 C07 01</t>
   </si>
   <si>
     <t>007957</t>
@@ -59,25 +272,166 @@
     <t>PAQUET DE 3,06M2 - DIM 1288X198X7MM</t>
   </si>
   <si>
-    <t>M2</t>
-  </si>
-  <si>
-    <t>014537</t>
-  </si>
-  <si>
-    <t>VINYLE RD300S 7326 CHENE BH 228X1290X5,5</t>
-  </si>
-  <si>
-    <t>REF5941007326 PAQUET DE 2,06M2 MEISTER</t>
-  </si>
-  <si>
-    <t>009247</t>
-  </si>
-  <si>
-    <t>MODULAR ONE CHENE PURE TEXTURE BOIS</t>
-  </si>
-  <si>
-    <t>PQT DE 2,493M2 DIM1285X194X8MM PARADOR</t>
+    <t>A1 01 C07 02</t>
+  </si>
+  <si>
+    <t>012954</t>
+  </si>
+  <si>
+    <t>SOL STRATIFIE LC55 CHENE MARRAKECH 6396</t>
+  </si>
+  <si>
+    <t>A1 01 C07 03</t>
+  </si>
+  <si>
+    <t>007961</t>
+  </si>
+  <si>
+    <t>SOL STRATIFIE LC55 CHENE FISSURE T 6439</t>
+  </si>
+  <si>
+    <t>A1 01 C08 01</t>
+  </si>
+  <si>
+    <t>012872</t>
+  </si>
+  <si>
+    <t>SOL STRATIFIE LL150S CHENE FISSURE 6258</t>
+  </si>
+  <si>
+    <t>PAQUET DE 2,26M2 - DIM 2052X220X10 MM</t>
+  </si>
+  <si>
+    <t>A1 01 C09 01</t>
+  </si>
+  <si>
+    <t>012873</t>
+  </si>
+  <si>
+    <t>SOL STRATIFIE LL150S CHENE HANGAR 6259</t>
+  </si>
+  <si>
+    <t>A1 01 C10 01</t>
+  </si>
+  <si>
+    <t>009326</t>
+  </si>
+  <si>
+    <t>PARQUET LOFT PRO CHENE RU HUILE INCOLORE</t>
+  </si>
+  <si>
+    <t>PQT DE 1,914M2 145X12X1000-2200 GO2 R+L</t>
+  </si>
+  <si>
+    <t>A1 01 C11 01</t>
+  </si>
+  <si>
+    <t>017017</t>
+  </si>
+  <si>
+    <t>PARQUET LOFT PRO CHENE DOLOMITES RU/CA</t>
+  </si>
+  <si>
+    <t>180X12X600-2200 PAQT 2,376M2 VERNI INCOL</t>
+  </si>
+  <si>
+    <t>A1 01 C12 01</t>
+  </si>
+  <si>
+    <t>012651</t>
+  </si>
+  <si>
+    <t>BLOC PORTE ISOLANT CL B 67X56 73X204 GP</t>
+  </si>
+  <si>
+    <t>A1 01 C13 01</t>
+  </si>
+  <si>
+    <t>012652</t>
+  </si>
+  <si>
+    <t>BLOC PORTE ISOLANT CL B 67X56 73X204 DP</t>
+  </si>
+  <si>
+    <t>A1 01 D02 01</t>
+  </si>
+  <si>
+    <t>007930</t>
+  </si>
+  <si>
+    <t>SOUS COUCHE QUALIFOAM 2 MM 19 DB</t>
+  </si>
+  <si>
+    <t>ROULEAU DE 15M2 REF3208 POLYANE INTEGRE</t>
+  </si>
+  <si>
+    <t>A1 01 D02 02</t>
+  </si>
+  <si>
+    <t>007710</t>
+  </si>
+  <si>
+    <t>SOUS COUCHE ISOLSOUND ALU 2 MM 18DB</t>
+  </si>
+  <si>
+    <t>ROULEAU DE 15M2 REF3392 POLYANE INTEGRE</t>
+  </si>
+  <si>
+    <t>A1 01 D02 03</t>
+  </si>
+  <si>
+    <t>019584</t>
+  </si>
+  <si>
+    <t>SOUS COUCHE TRAMISOL FIBRE ROULEAU 15M2</t>
+  </si>
+  <si>
+    <t>REF2912680000 SANS POLYANE  EP 3,5MM</t>
+  </si>
+  <si>
+    <t>A1 01 D05 01</t>
+  </si>
+  <si>
+    <t>013738</t>
+  </si>
+  <si>
+    <t>ESCALIER ESCAMOTABLE ISOCLIC 120X60</t>
+  </si>
+  <si>
+    <t>HTMAX=2M72 TRAPPE 56 MM CAISSON U :</t>
+  </si>
+  <si>
+    <t>A1 01 D05 02</t>
+  </si>
+  <si>
+    <t>013739</t>
+  </si>
+  <si>
+    <t>ESCALIER ESCAMOTABLE ISOCLIC 140X70</t>
+  </si>
+  <si>
+    <t>A1 01 D06 02</t>
+  </si>
+  <si>
+    <t>009246</t>
+  </si>
+  <si>
+    <t>MODULAR ONE PURE NATUREL TEXTURE BOIS</t>
+  </si>
+  <si>
+    <t>A1 01 D06 03</t>
+  </si>
+  <si>
+    <t>012852</t>
+  </si>
+  <si>
+    <t>SOL STRATIFIE LD150 CHENE CHIANTI 6392</t>
+  </si>
+  <si>
+    <t>PAQUET DE 2,55M2 - DIM 1288X198X8MM</t>
+  </si>
+  <si>
+    <t>A1 01 D07 01</t>
   </si>
   <si>
     <t>012860</t>
@@ -86,40 +440,49 @@
     <t>SOL STRATIFIE LD150 CHENE TAVERNA 6428</t>
   </si>
   <si>
-    <t>PAQUET DE 2,55M2 - DIM 1288X198X8MM</t>
-  </si>
-  <si>
-    <t>004864</t>
-  </si>
-  <si>
-    <t>PARQUET LOFT MOUNT CHENE APENNINES RU/CA</t>
-  </si>
-  <si>
-    <t>PAQUET DE 2,075M2 1820X190X14 HUILE GO4</t>
-  </si>
-  <si>
-    <t>012654</t>
-  </si>
-  <si>
-    <t>BLOC PORTE ISOLANT CL B 67X56 83X204 DP</t>
-  </si>
-  <si>
-    <t>CHANT DROIT S3PT PERF+ AXE 50 JB FILME</t>
-  </si>
-  <si>
-    <t>UN</t>
-  </si>
-  <si>
-    <t>009246</t>
-  </si>
-  <si>
-    <t>MODULAR ONE PURE NATUREL TEXTURE BOIS</t>
-  </si>
-  <si>
-    <t>007961</t>
-  </si>
-  <si>
-    <t>SOL STRATIFIE LC55 CHENE FISSURE T 6439</t>
+    <t>A1 01 D07 02</t>
+  </si>
+  <si>
+    <t>012861</t>
+  </si>
+  <si>
+    <t>SOL STRATIFIE LD150 CHENE BLANC LES 6181</t>
+  </si>
+  <si>
+    <t>A1 01 D07 03</t>
+  </si>
+  <si>
+    <t>007955</t>
+  </si>
+  <si>
+    <t>SOL STRATIFIE LC55 CHENE NATURE 6067</t>
+  </si>
+  <si>
+    <t>A1 01 D08 01</t>
+  </si>
+  <si>
+    <t>016006</t>
+  </si>
+  <si>
+    <t>PLINTHE PREPEINTE SX163 2000X102X13MM</t>
+  </si>
+  <si>
+    <t>DUROPOLYMER IMPUTRESCIBLE</t>
+  </si>
+  <si>
+    <t>A1 01 D09 01</t>
+  </si>
+  <si>
+    <t>006807</t>
+  </si>
+  <si>
+    <t>PLINTHE MDF MELAMINE BLANC 2400X80X14</t>
+  </si>
+  <si>
+    <t>BORD RD REF.007184 PAR PQT DE 5 PLINTHES</t>
+  </si>
+  <si>
+    <t>A1 01 D10 01</t>
   </si>
   <si>
     <t>004529</t>
@@ -131,115 +494,7 @@
     <t>BORD DROIT REF.9800 PQT DE 10 PLINTHES</t>
   </si>
   <si>
-    <t>009248</t>
-  </si>
-  <si>
-    <t>PARQUET LOFT PRO CHENE ARZON RU/CA HUIL</t>
-  </si>
-  <si>
-    <t>180X12X1000-2000 PAQT 2,376M2 INCOLORE</t>
-  </si>
-  <si>
-    <t>008229</t>
-  </si>
-  <si>
-    <t>SOUS COUCHE ISOLSOUND HD+ 2 MM 18 DB</t>
-  </si>
-  <si>
-    <t>ROULEAU DE 7,50M2REF3393 POLYANE INTEGRE</t>
-  </si>
-  <si>
-    <t>RL(X)</t>
-  </si>
-  <si>
-    <t>012873</t>
-  </si>
-  <si>
-    <t>SOL STRATIFIE LL150S CHENE HANGAR 6259</t>
-  </si>
-  <si>
-    <t>PAQUET DE 2,26M2 - DIM 2052X220X10 MM</t>
-  </si>
-  <si>
-    <t>012651</t>
-  </si>
-  <si>
-    <t>BLOC PORTE ISOLANT CL B 67X56 73X204 GP</t>
-  </si>
-  <si>
-    <t>012852</t>
-  </si>
-  <si>
-    <t>SOL STRATIFIE LD150 CHENE CHIANTI 6392</t>
-  </si>
-  <si>
-    <t>012861</t>
-  </si>
-  <si>
-    <t>SOL STRATIFIE LD150 CHENE BLANC LES 6181</t>
-  </si>
-  <si>
-    <t>012656</t>
-  </si>
-  <si>
-    <t>BLOC PORTE ISOLANT CL B 67X56 93X204 DP</t>
-  </si>
-  <si>
-    <t>006700</t>
-  </si>
-  <si>
-    <t>STRATIFIE BASIC 400V CHENE POLI TEXT M S</t>
-  </si>
-  <si>
-    <t>REF1426542 PAQUET DE 2,493M2 PARADOR</t>
-  </si>
-  <si>
-    <t>013741</t>
-  </si>
-  <si>
-    <t>ESCALIER ESCAMOTABLE ECOWOOD36 140X70</t>
-  </si>
-  <si>
-    <t>HTMAX=2M80 TRAPPE 36 MM CAISSON U :</t>
-  </si>
-  <si>
-    <t>BANDES PHALTEX 1200X48X10 MM</t>
-  </si>
-  <si>
-    <t>PAQUET DE 50 BANDES STEICO</t>
-  </si>
-  <si>
-    <t>PQT</t>
-  </si>
-  <si>
-    <t>020494</t>
-  </si>
-  <si>
-    <t>ESCALIER ESCAMOTABLE ECOWOOD40 120X60</t>
-  </si>
-  <si>
-    <t>HTMAX=2M84 TRAPPE 40 MM CAISSON U :</t>
-  </si>
-  <si>
-    <t>012954</t>
-  </si>
-  <si>
-    <t>SOL STRATIFIE LC55 CHENE MARRAKECH 6396</t>
-  </si>
-  <si>
-    <t>006698</t>
-  </si>
-  <si>
-    <t>STRATIFIE BASIC 400V CHENE GRIS LUMIERE</t>
-  </si>
-  <si>
-    <t>REF1426530 PAQUET DE 2,493M2 PARADOR</t>
-  </si>
-  <si>
-    <t>007955</t>
-  </si>
-  <si>
-    <t>SOL STRATIFIE LC55 CHENE NATURE 6067</t>
+    <t>A1 01 D11 01</t>
   </si>
   <si>
     <t>015528</t>
@@ -251,37 +506,7 @@
     <t>BORD DROIT G007037 PAQUET DE 10 PLINTHES</t>
   </si>
   <si>
-    <t>013739</t>
-  </si>
-  <si>
-    <t>ESCALIER ESCAMOTABLE ISOCLIC 140X70</t>
-  </si>
-  <si>
-    <t>HTMAX=2M72 TRAPPE 56 MM CAISSON U :</t>
-  </si>
-  <si>
-    <t>009326</t>
-  </si>
-  <si>
-    <t>PARQUET LOFT PRO CHENE RU HUILE INCOLORE</t>
-  </si>
-  <si>
-    <t>PQT DE 1,914M2 145X12X1000-2200 GO2 R+L</t>
-  </si>
-  <si>
-    <t>010427</t>
-  </si>
-  <si>
-    <t>MODULAR ONE CHENE URBAN CHAULE GRIS</t>
-  </si>
-  <si>
-    <t>007356</t>
-  </si>
-  <si>
-    <t>STRATIFIE BASIC 400V CHENE HORIZON NATUR</t>
-  </si>
-  <si>
-    <t>REF1593797 PAQUET DE 2,493M2 PARADOR</t>
+    <t>A1 01 D12 01</t>
   </si>
   <si>
     <t>008641</t>
@@ -291,108 +516,6 @@
   </si>
   <si>
     <t>BORD DROIT REF. 0007 PAQT DE 5 PLINTHES</t>
-  </si>
-  <si>
-    <t>017017</t>
-  </si>
-  <si>
-    <t>PARQUET LOFT PRO CHENE DOLOMITES RU/CA</t>
-  </si>
-  <si>
-    <t>180X12X600-2200 PAQT 2,376M2 VERNI INCOL</t>
-  </si>
-  <si>
-    <t>007930</t>
-  </si>
-  <si>
-    <t>SOUS COUCHE QUALIFOAM 2 MM 19 DB</t>
-  </si>
-  <si>
-    <t>ROULEAU DE 15M2 REF3208 POLYANE INTEGRE</t>
-  </si>
-  <si>
-    <t>012653</t>
-  </si>
-  <si>
-    <t>BLOC PORTE ISOLANT CL B 67X56 83X204 GP</t>
-  </si>
-  <si>
-    <t>006807</t>
-  </si>
-  <si>
-    <t>PLINTHE MDF MELAMINE BLANC 2400X80X14</t>
-  </si>
-  <si>
-    <t>BORD RD REF.007184 PAR PQT DE 5 PLINTHES</t>
-  </si>
-  <si>
-    <t>006852</t>
-  </si>
-  <si>
-    <t>PARQUET LOFT PRO CHENE RU BROSSE VERNI</t>
-  </si>
-  <si>
-    <t>PQT DE 1,914M2 145X12X600-2200 G02 R+L</t>
-  </si>
-  <si>
-    <t>007710</t>
-  </si>
-  <si>
-    <t>SOUS COUCHE ISOLSOUND ALU 2 MM 18DB</t>
-  </si>
-  <si>
-    <t>ROULEAU DE 15M2 REF3392 POLYANE INTEGRE</t>
-  </si>
-  <si>
-    <t>013738</t>
-  </si>
-  <si>
-    <t>ESCALIER ESCAMOTABLE ISOCLIC 120X60</t>
-  </si>
-  <si>
-    <t>012655</t>
-  </si>
-  <si>
-    <t>BLOC PORTE ISOLANT CL B 67X56 93X204 GP</t>
-  </si>
-  <si>
-    <t>019584</t>
-  </si>
-  <si>
-    <t>SOUS COUCHE TRAMISOL FIBRE ROULEAU 15M2</t>
-  </si>
-  <si>
-    <t>REF2912680000 SANS POLYANE  EP 3,5MM</t>
-  </si>
-  <si>
-    <t>016006</t>
-  </si>
-  <si>
-    <t>PLINTHE PREPEINTE SX163 2000X102X13MM</t>
-  </si>
-  <si>
-    <t>DUROPOLYMER IMPUTRESCIBLE</t>
-  </si>
-  <si>
-    <t>012872</t>
-  </si>
-  <si>
-    <t>SOL STRATIFIE LL150S CHENE FISSURE 6258</t>
-  </si>
-  <si>
-    <t>012918</t>
-  </si>
-  <si>
-    <t>SOL STRATIFIE LD250 CHENE CAMPAGN 6843</t>
-  </si>
-  <si>
-    <t>PAQUET DE 1,70M2 - DIM 1287X220X10 MM</t>
-  </si>
-  <si>
-    <t>012652</t>
-  </si>
-  <si>
-    <t>BLOC PORTE ISOLANT CL B 67X56 73X204 DP</t>
   </si>
 </sst>
 </file>
@@ -791,16 +914,16 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="G3" t="s">
         <v>14</v>
@@ -808,169 +931,169 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G4" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="G5" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="G6" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="G7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="G8" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="D9" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="G9" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="D10" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="G10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="D11" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="G11" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="D12" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="G12" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="C13" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="D13" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="G13" t="s">
         <v>14</v>
@@ -978,33 +1101,33 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" t="s">
-        <v>48</v>
+        <v>58</v>
+      </c>
+      <c r="B14">
+        <v>30313120</v>
       </c>
       <c r="C14" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="D14" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="G14" t="s">
-        <v>30</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>62</v>
       </c>
       <c r="B15" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="C15" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="D15" t="s">
-        <v>23</v>
+        <v>65</v>
       </c>
       <c r="G15" t="s">
         <v>14</v>
@@ -1012,16 +1135,16 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="B16" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="D16" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="G16" t="s">
         <v>14</v>
@@ -1029,186 +1152,186 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="B17" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="C17" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="D17" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="G17" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>74</v>
       </c>
       <c r="B18" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="C18" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="D18" t="s">
-        <v>58</v>
+        <v>26</v>
       </c>
       <c r="G18" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>10</v>
+        <v>77</v>
       </c>
       <c r="B19" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="C19" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="D19" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="G19" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>10</v>
-      </c>
-      <c r="B20">
-        <v>30313120</v>
+        <v>81</v>
+      </c>
+      <c r="B20" t="s">
+        <v>82</v>
       </c>
       <c r="C20" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="D20" t="s">
-        <v>63</v>
+        <v>84</v>
       </c>
       <c r="G20" t="s">
-        <v>64</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>10</v>
+        <v>85</v>
       </c>
       <c r="B21" t="s">
-        <v>65</v>
+        <v>86</v>
       </c>
       <c r="C21" t="s">
-        <v>66</v>
+        <v>87</v>
       </c>
       <c r="D21" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="G21" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>88</v>
       </c>
       <c r="B22" t="s">
-        <v>68</v>
+        <v>89</v>
       </c>
       <c r="C22" t="s">
-        <v>69</v>
+        <v>90</v>
       </c>
       <c r="D22" t="s">
-        <v>13</v>
+        <v>84</v>
       </c>
       <c r="G22" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="B23" t="s">
-        <v>70</v>
+        <v>92</v>
       </c>
       <c r="C23" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="D23" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="G23" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" t="s">
-        <v>10</v>
+        <v>95</v>
       </c>
       <c r="B24" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="C24" t="s">
-        <v>74</v>
+        <v>97</v>
       </c>
       <c r="D24" t="s">
-        <v>13</v>
+        <v>94</v>
       </c>
       <c r="G24" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" t="s">
-        <v>10</v>
+        <v>98</v>
       </c>
       <c r="B25" t="s">
-        <v>75</v>
+        <v>99</v>
       </c>
       <c r="C25" t="s">
-        <v>76</v>
+        <v>100</v>
       </c>
       <c r="D25" t="s">
-        <v>77</v>
+        <v>101</v>
       </c>
       <c r="G25" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
       <c r="B26" t="s">
-        <v>78</v>
+        <v>103</v>
       </c>
       <c r="C26" t="s">
-        <v>79</v>
+        <v>104</v>
       </c>
       <c r="D26" t="s">
-        <v>80</v>
+        <v>105</v>
       </c>
       <c r="G26" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" t="s">
-        <v>10</v>
+        <v>106</v>
       </c>
       <c r="B27" t="s">
-        <v>81</v>
+        <v>107</v>
       </c>
       <c r="C27" t="s">
-        <v>82</v>
+        <v>108</v>
       </c>
       <c r="D27" t="s">
-        <v>83</v>
+        <v>13</v>
       </c>
       <c r="G27" t="s">
         <v>14</v>
@@ -1216,16 +1339,16 @@
     </row>
     <row r="28" spans="1:10">
       <c r="A28" t="s">
-        <v>10</v>
+        <v>109</v>
       </c>
       <c r="B28" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
       <c r="C28" t="s">
-        <v>85</v>
+        <v>111</v>
       </c>
       <c r="D28" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="G28" t="s">
         <v>14</v>
@@ -1233,16 +1356,16 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" t="s">
-        <v>10</v>
+        <v>112</v>
       </c>
       <c r="B29" t="s">
-        <v>86</v>
+        <v>113</v>
       </c>
       <c r="C29" t="s">
-        <v>87</v>
+        <v>114</v>
       </c>
       <c r="D29" t="s">
-        <v>88</v>
+        <v>115</v>
       </c>
       <c r="G29" t="s">
         <v>14</v>
@@ -1250,203 +1373,203 @@
     </row>
     <row r="30" spans="1:10">
       <c r="A30" t="s">
-        <v>10</v>
+        <v>116</v>
       </c>
       <c r="B30" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="C30" t="s">
-        <v>90</v>
+        <v>118</v>
       </c>
       <c r="D30" t="s">
-        <v>91</v>
+        <v>119</v>
       </c>
       <c r="G30" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" t="s">
-        <v>10</v>
+        <v>120</v>
       </c>
       <c r="B31" t="s">
-        <v>92</v>
+        <v>121</v>
       </c>
       <c r="C31" t="s">
-        <v>93</v>
+        <v>122</v>
       </c>
       <c r="D31" t="s">
-        <v>94</v>
+        <v>123</v>
       </c>
       <c r="G31" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" t="s">
-        <v>10</v>
+        <v>124</v>
       </c>
       <c r="B32" t="s">
-        <v>95</v>
+        <v>125</v>
       </c>
       <c r="C32" t="s">
-        <v>96</v>
+        <v>126</v>
       </c>
       <c r="D32" t="s">
-        <v>97</v>
+        <v>127</v>
       </c>
       <c r="G32" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:10">
       <c r="A33" t="s">
-        <v>10</v>
+        <v>128</v>
       </c>
       <c r="B33" t="s">
-        <v>98</v>
+        <v>129</v>
       </c>
       <c r="C33" t="s">
-        <v>99</v>
+        <v>130</v>
       </c>
       <c r="D33" t="s">
-        <v>29</v>
+        <v>127</v>
       </c>
       <c r="G33" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:10">
       <c r="A34" t="s">
-        <v>10</v>
+        <v>131</v>
       </c>
       <c r="B34" t="s">
-        <v>100</v>
+        <v>132</v>
       </c>
       <c r="C34" t="s">
-        <v>101</v>
+        <v>133</v>
       </c>
       <c r="D34" t="s">
-        <v>102</v>
+        <v>26</v>
       </c>
       <c r="G34" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="35" spans="1:10">
       <c r="A35" t="s">
-        <v>10</v>
+        <v>134</v>
       </c>
       <c r="B35" t="s">
-        <v>103</v>
+        <v>135</v>
       </c>
       <c r="C35" t="s">
-        <v>104</v>
+        <v>136</v>
       </c>
       <c r="D35" t="s">
-        <v>105</v>
+        <v>137</v>
       </c>
       <c r="G35" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" t="s">
-        <v>10</v>
+        <v>138</v>
       </c>
       <c r="B36" t="s">
-        <v>106</v>
+        <v>139</v>
       </c>
       <c r="C36" t="s">
-        <v>107</v>
+        <v>140</v>
       </c>
       <c r="D36" t="s">
-        <v>108</v>
+        <v>137</v>
       </c>
       <c r="G36" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" t="s">
-        <v>10</v>
+        <v>141</v>
       </c>
       <c r="B37" t="s">
-        <v>109</v>
+        <v>142</v>
       </c>
       <c r="C37" t="s">
-        <v>110</v>
+        <v>143</v>
       </c>
       <c r="D37" t="s">
-        <v>80</v>
+        <v>137</v>
       </c>
       <c r="G37" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="38" spans="1:10">
       <c r="A38" t="s">
-        <v>10</v>
+        <v>144</v>
       </c>
       <c r="B38" t="s">
-        <v>111</v>
+        <v>145</v>
       </c>
       <c r="C38" t="s">
-        <v>112</v>
+        <v>146</v>
       </c>
       <c r="D38" t="s">
-        <v>29</v>
+        <v>84</v>
       </c>
       <c r="G38" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" t="s">
-        <v>10</v>
+        <v>147</v>
       </c>
       <c r="B39" t="s">
-        <v>113</v>
+        <v>148</v>
       </c>
       <c r="C39" t="s">
-        <v>114</v>
+        <v>149</v>
       </c>
       <c r="D39" t="s">
-        <v>115</v>
+        <v>150</v>
       </c>
       <c r="G39" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" t="s">
-        <v>10</v>
+        <v>151</v>
       </c>
       <c r="B40" t="s">
-        <v>116</v>
+        <v>152</v>
       </c>
       <c r="C40" t="s">
-        <v>117</v>
+        <v>153</v>
       </c>
       <c r="D40" t="s">
-        <v>118</v>
+        <v>154</v>
       </c>
       <c r="G40" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
     </row>
     <row r="41" spans="1:10">
       <c r="A41" t="s">
-        <v>10</v>
+        <v>155</v>
       </c>
       <c r="B41" t="s">
-        <v>119</v>
+        <v>156</v>
       </c>
       <c r="C41" t="s">
-        <v>120</v>
+        <v>157</v>
       </c>
       <c r="D41" t="s">
-        <v>47</v>
+        <v>158</v>
       </c>
       <c r="G41" t="s">
         <v>14</v>
@@ -1454,16 +1577,16 @@
     </row>
     <row r="42" spans="1:10">
       <c r="A42" t="s">
-        <v>10</v>
+        <v>159</v>
       </c>
       <c r="B42" t="s">
-        <v>121</v>
+        <v>160</v>
       </c>
       <c r="C42" t="s">
-        <v>122</v>
+        <v>161</v>
       </c>
       <c r="D42" t="s">
-        <v>123</v>
+        <v>162</v>
       </c>
       <c r="G42" t="s">
         <v>14</v>
@@ -1471,19 +1594,19 @@
     </row>
     <row r="43" spans="1:10">
       <c r="A43" t="s">
-        <v>10</v>
+        <v>163</v>
       </c>
       <c r="B43" t="s">
-        <v>124</v>
+        <v>164</v>
       </c>
       <c r="C43" t="s">
-        <v>125</v>
+        <v>165</v>
       </c>
       <c r="D43" t="s">
-        <v>29</v>
+        <v>166</v>
       </c>
       <c r="G43" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>